<commit_message>
Update Times for `Abschlussbericht`
</commit_message>
<xml_diff>
--- a/documentation/timemanagment/neuner-timemanagment.xlsx
+++ b/documentation/timemanagment/neuner-timemanagment.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mfn\git\g6t3\documentation\timemanagment\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{20744E71-613B-4B36-85BD-6EFF8428B59B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{724F841A-B7E6-44D0-99EB-37196EFDEFE8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
+    <workbookView xWindow="2895" yWindow="2895" windowWidth="21600" windowHeight="11385" xr2:uid="{6E71D473-8E99-584F-9CE7-0EC5B1B78532}"/>
   </bookViews>
   <sheets>
     <sheet name="Datenerfassung" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="164" uniqueCount="66">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="68">
   <si>
     <t>Anmerkung</t>
   </si>
@@ -244,6 +244,12 @@
   </si>
   <si>
     <t>Update Timemanagment</t>
+  </si>
+  <si>
+    <t>Clean Up</t>
+  </si>
+  <si>
+    <t>Review Cube MR</t>
   </si>
 </sst>
 </file>
@@ -674,10 +680,10 @@
   <dimension ref="A1:F1001"/>
   <sheetViews>
     <sheetView tabSelected="1" zoomScaleNormal="100" workbookViewId="0">
-      <pane xSplit="2" ySplit="1" topLeftCell="C47" activePane="bottomRight" state="frozen"/>
+      <pane xSplit="2" ySplit="1" topLeftCell="C68" activePane="bottomRight" state="frozen"/>
       <selection pane="topRight" activeCell="C1" sqref="C1"/>
       <selection pane="bottomLeft" activeCell="A2" sqref="A2"/>
-      <selection pane="bottomRight" activeCell="C75" sqref="C75"/>
+      <selection pane="bottomRight" activeCell="D79" sqref="D79"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="11" defaultRowHeight="15.75"/>
@@ -1747,14 +1753,32 @@
       </c>
     </row>
     <row r="77" spans="1:4">
-      <c r="A77" s="8"/>
-      <c r="B77" s="7"/>
-      <c r="D77" s="3"/>
+      <c r="A77" s="8">
+        <v>44365</v>
+      </c>
+      <c r="B77" s="7">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C77" t="s">
+        <v>4</v>
+      </c>
+      <c r="D77" s="3" t="s">
+        <v>66</v>
+      </c>
     </row>
     <row r="78" spans="1:4">
-      <c r="A78" s="8"/>
-      <c r="B78" s="7"/>
-      <c r="D78" s="3"/>
+      <c r="A78" s="8">
+        <v>44365</v>
+      </c>
+      <c r="B78" s="7">
+        <v>2.0833333333333332E-2</v>
+      </c>
+      <c r="C78" t="s">
+        <v>13</v>
+      </c>
+      <c r="D78" s="3" t="s">
+        <v>67</v>
+      </c>
     </row>
     <row r="79" spans="1:4">
       <c r="A79" s="8"/>

</xml_diff>